<commit_message>
Test to update file
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_B-NewTechs_TRA_Trans.xlsx
+++ b/SubRES_TMPL/SubRes_B-NewTechs_TRA_Trans.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\Veda_models\City_TRA_STHLM\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GabGren\Work Folders\Documents\TransportElModellSthlm\SimpleModel\City_TRA_STHLM\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1607C67-6A38-4094-BB51-686D1F6C519A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FC893F4-0864-4DD6-A013-5A15D1B5DB21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1812" yWindow="1812" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1425" windowWidth="28800" windowHeight="15375" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Param_Transformation" sheetId="3" r:id="rId1"/>
@@ -3721,25 +3721,25 @@
       <selection pane="bottomLeft" activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" customWidth="1"/>
-    <col min="7" max="7" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E1">
         <f>FILL!F1+1</f>
         <v>2020</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
         <v>24</v>
       </c>
@@ -3753,7 +3753,7 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="11" t="s">
         <v>4</v>
       </c>
@@ -3785,7 +3785,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="13" t="s">
@@ -3799,7 +3799,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="str">
@@ -3825,7 +3825,7 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="str">
@@ -3851,7 +3851,7 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="str">
@@ -3877,7 +3877,7 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="str">
@@ -3903,7 +3903,7 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="str">
@@ -3928,7 +3928,7 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="str">
@@ -3953,7 +3953,7 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1" t="str">
@@ -3979,7 +3979,7 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="str">
@@ -4005,7 +4005,7 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="str">
@@ -4031,7 +4031,7 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="str">
@@ -4057,7 +4057,7 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="str">
@@ -4083,7 +4083,7 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="str">
@@ -4109,7 +4109,7 @@
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1" t="str">
@@ -4135,7 +4135,7 @@
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1" t="str">
@@ -4161,7 +4161,7 @@
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1" t="str">
@@ -4187,7 +4187,7 @@
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1" t="str">
@@ -4213,7 +4213,7 @@
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1" t="str">
@@ -4239,7 +4239,7 @@
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1" t="str">
@@ -4265,7 +4265,7 @@
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1" t="str">
@@ -4291,7 +4291,7 @@
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1" t="str">
@@ -4317,7 +4317,7 @@
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" s="14"/>
       <c r="C26" s="14"/>
       <c r="D26" s="14" t="str">
@@ -4343,7 +4343,7 @@
       <c r="J26" s="14"/>
       <c r="K26" s="14"/>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C27" s="1"/>
       <c r="D27" s="13" t="s">
         <v>27</v>
@@ -4355,7 +4355,7 @@
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
         <v>16</v>
       </c>
@@ -4383,7 +4383,7 @@
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
         <v>16</v>
       </c>
@@ -4411,7 +4411,7 @@
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
         <v>16</v>
       </c>
@@ -4439,7 +4439,7 @@
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>16</v>
       </c>
@@ -4467,7 +4467,7 @@
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>16</v>
       </c>
@@ -4484,7 +4484,7 @@
       </c>
       <c r="F32" s="25">
         <f>FILL!Y31</f>
-        <v>5.8509000000000002</v>
+        <v>10.5219</v>
       </c>
       <c r="G32" s="24" t="s">
         <v>65</v>
@@ -4494,7 +4494,7 @@
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>16</v>
       </c>
@@ -4521,7 +4521,7 @@
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
         <v>16</v>
       </c>
@@ -4538,7 +4538,7 @@
       </c>
       <c r="F34" s="25">
         <f>FILL!Y33</f>
-        <v>6.7997576454545499</v>
+        <v>13.5995152909091</v>
       </c>
       <c r="G34" s="1" t="str">
         <f>FILL!G33&amp;",-*00"</f>
@@ -4549,7 +4549,7 @@
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
         <v>16</v>
       </c>
@@ -4577,7 +4577,7 @@
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
         <v>16</v>
       </c>
@@ -4605,7 +4605,7 @@
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
         <v>16</v>
       </c>
@@ -4633,7 +4633,7 @@
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
         <v>16</v>
       </c>
@@ -4661,7 +4661,7 @@
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
     </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
         <v>16</v>
       </c>
@@ -4689,7 +4689,7 @@
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
     </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
         <v>16</v>
       </c>
@@ -4717,7 +4717,7 @@
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
     </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
         <v>16</v>
       </c>
@@ -4745,7 +4745,7 @@
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
     </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
         <v>16</v>
       </c>
@@ -4773,7 +4773,7 @@
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
     </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
         <v>16</v>
       </c>
@@ -4801,7 +4801,7 @@
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
     </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
         <v>16</v>
       </c>
@@ -4829,7 +4829,7 @@
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
     </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
         <v>16</v>
       </c>
@@ -4857,7 +4857,7 @@
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
     </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
         <v>16</v>
       </c>
@@ -4885,7 +4885,7 @@
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
     </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B47" s="16" t="s">
         <v>16</v>
       </c>
@@ -4913,7 +4913,7 @@
       <c r="J47" s="16"/>
       <c r="K47" s="1"/>
     </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B48" s="14" t="s">
         <v>16</v>
       </c>
@@ -4941,7 +4941,7 @@
       <c r="J48" s="14"/>
       <c r="K48" s="14"/>
     </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
@@ -4953,7 +4953,7 @@
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
     </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -4965,7 +4965,7 @@
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
     </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B51" s="10" t="s">
         <v>64</v>
       </c>
@@ -4979,7 +4979,7 @@
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
     </row>
-    <row r="52" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="11" t="s">
         <v>4</v>
       </c>
@@ -5011,7 +5011,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="13" t="s">
@@ -5025,7 +5025,7 @@
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
     </row>
-    <row r="54" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1" t="str">
@@ -5048,7 +5048,7 @@
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
     </row>
-    <row r="55" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1" t="str">
@@ -5071,7 +5071,7 @@
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
     </row>
-    <row r="56" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1" t="str">
@@ -5094,7 +5094,7 @@
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
     </row>
-    <row r="57" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1" t="str">
@@ -5117,7 +5117,7 @@
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
     </row>
-    <row r="58" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1" t="str">
@@ -5140,7 +5140,7 @@
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
     </row>
-    <row r="59" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1" t="str">
@@ -5163,7 +5163,7 @@
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
     </row>
-    <row r="60" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1" t="str">
@@ -5186,7 +5186,7 @@
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
     </row>
-    <row r="61" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1" t="str">
@@ -5209,7 +5209,7 @@
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
     </row>
-    <row r="62" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1" t="str">
@@ -5232,7 +5232,7 @@
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
     </row>
-    <row r="63" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1" t="str">
@@ -5255,7 +5255,7 @@
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
     </row>
-    <row r="64" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1" t="str">
@@ -5278,7 +5278,7 @@
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
     </row>
-    <row r="65" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1" t="str">
@@ -5301,7 +5301,7 @@
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
     </row>
-    <row r="66" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1" t="str">
@@ -5324,7 +5324,7 @@
       <c r="J66" s="1"/>
       <c r="K66" s="1"/>
     </row>
-    <row r="67" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1" t="str">
@@ -5347,7 +5347,7 @@
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
     </row>
-    <row r="68" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1" t="str">
@@ -5370,7 +5370,7 @@
       <c r="J68" s="1"/>
       <c r="K68" s="1"/>
     </row>
-    <row r="69" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1" t="str">
@@ -5393,7 +5393,7 @@
       <c r="J69" s="1"/>
       <c r="K69" s="1"/>
     </row>
-    <row r="70" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1" t="str">
@@ -5416,7 +5416,7 @@
       <c r="J70" s="1"/>
       <c r="K70" s="1"/>
     </row>
-    <row r="71" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1" t="str">
@@ -5439,7 +5439,7 @@
       <c r="J71" s="1"/>
       <c r="K71" s="1"/>
     </row>
-    <row r="72" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1" t="str">
@@ -5462,7 +5462,7 @@
       <c r="J72" s="1"/>
       <c r="K72" s="1"/>
     </row>
-    <row r="73" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1" t="str">
@@ -5485,7 +5485,7 @@
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
     </row>
-    <row r="74" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B74" s="14"/>
       <c r="C74" s="14"/>
       <c r="D74" s="14" t="str">
@@ -5508,7 +5508,7 @@
       <c r="J74" s="14"/>
       <c r="K74" s="14"/>
     </row>
-    <row r="75" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C75" s="1"/>
       <c r="D75" s="13" t="s">
         <v>27</v>
@@ -5520,7 +5520,7 @@
       <c r="J75" s="1"/>
       <c r="K75" s="1"/>
     </row>
-    <row r="76" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B76" s="1" t="s">
         <v>16</v>
       </c>
@@ -5543,7 +5543,7 @@
       <c r="J76" s="1"/>
       <c r="K76" s="1"/>
     </row>
-    <row r="77" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B77" s="1" t="s">
         <v>16</v>
       </c>
@@ -5566,7 +5566,7 @@
       <c r="J77" s="1"/>
       <c r="K77" s="1"/>
     </row>
-    <row r="78" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B78" s="1" t="s">
         <v>16</v>
       </c>
@@ -5589,7 +5589,7 @@
       <c r="J78" s="1"/>
       <c r="K78" s="1"/>
     </row>
-    <row r="79" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B79" s="1" t="s">
         <v>16</v>
       </c>
@@ -5612,7 +5612,7 @@
       <c r="J79" s="1"/>
       <c r="K79" s="1"/>
     </row>
-    <row r="80" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B80" s="1" t="s">
         <v>16</v>
       </c>
@@ -5624,7 +5624,7 @@
       <c r="E80" s="16"/>
       <c r="F80" s="17">
         <f t="shared" ref="F80:G80" si="29">F32</f>
-        <v>5.8509000000000002</v>
+        <v>10.5219</v>
       </c>
       <c r="G80" s="1" t="str">
         <f t="shared" si="29"/>
@@ -5635,7 +5635,7 @@
       <c r="J80" s="1"/>
       <c r="K80" s="1"/>
     </row>
-    <row r="81" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B81" s="1" t="s">
         <v>16</v>
       </c>
@@ -5658,7 +5658,7 @@
       <c r="J81" s="1"/>
       <c r="K81" s="1"/>
     </row>
-    <row r="82" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B82" s="1" t="s">
         <v>16</v>
       </c>
@@ -5670,7 +5670,7 @@
       <c r="E82" s="16"/>
       <c r="F82" s="17">
         <f t="shared" ref="F82:G82" si="31">F34</f>
-        <v>6.7997576454545499</v>
+        <v>13.5995152909091</v>
       </c>
       <c r="G82" s="1" t="str">
         <f t="shared" si="31"/>
@@ -5681,7 +5681,7 @@
       <c r="J82" s="1"/>
       <c r="K82" s="1"/>
     </row>
-    <row r="83" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B83" s="1" t="s">
         <v>16</v>
       </c>
@@ -5704,7 +5704,7 @@
       <c r="J83" s="1"/>
       <c r="K83" s="1"/>
     </row>
-    <row r="84" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B84" s="1" t="s">
         <v>16</v>
       </c>
@@ -5727,7 +5727,7 @@
       <c r="J84" s="1"/>
       <c r="K84" s="1"/>
     </row>
-    <row r="85" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B85" s="1" t="s">
         <v>16</v>
       </c>
@@ -5750,7 +5750,7 @@
       <c r="J85" s="1"/>
       <c r="K85" s="1"/>
     </row>
-    <row r="86" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B86" s="1" t="s">
         <v>16</v>
       </c>
@@ -5773,7 +5773,7 @@
       <c r="J86" s="1"/>
       <c r="K86" s="1"/>
     </row>
-    <row r="87" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B87" s="1" t="s">
         <v>16</v>
       </c>
@@ -5796,7 +5796,7 @@
       <c r="J87" s="1"/>
       <c r="K87" s="1"/>
     </row>
-    <row r="88" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B88" s="1" t="s">
         <v>16</v>
       </c>
@@ -5819,7 +5819,7 @@
       <c r="J88" s="1"/>
       <c r="K88" s="1"/>
     </row>
-    <row r="89" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B89" s="1" t="s">
         <v>16</v>
       </c>
@@ -5842,7 +5842,7 @@
       <c r="J89" s="1"/>
       <c r="K89" s="1"/>
     </row>
-    <row r="90" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B90" s="1" t="s">
         <v>16</v>
       </c>
@@ -5865,7 +5865,7 @@
       <c r="J90" s="1"/>
       <c r="K90" s="1"/>
     </row>
-    <row r="91" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B91" s="1" t="s">
         <v>16</v>
       </c>
@@ -5888,7 +5888,7 @@
       <c r="J91" s="1"/>
       <c r="K91" s="1"/>
     </row>
-    <row r="92" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B92" s="1" t="s">
         <v>16</v>
       </c>
@@ -5911,7 +5911,7 @@
       <c r="J92" s="1"/>
       <c r="K92" s="1"/>
     </row>
-    <row r="93" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B93" s="1" t="s">
         <v>16</v>
       </c>
@@ -5934,7 +5934,7 @@
       <c r="J93" s="1"/>
       <c r="K93" s="1"/>
     </row>
-    <row r="94" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B94" s="1" t="s">
         <v>16</v>
       </c>
@@ -5957,7 +5957,7 @@
       <c r="J94" s="1"/>
       <c r="K94" s="1"/>
     </row>
-    <row r="95" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B95" s="16" t="s">
         <v>16</v>
       </c>
@@ -5980,7 +5980,7 @@
       <c r="J95" s="16"/>
       <c r="K95" s="1"/>
     </row>
-    <row r="96" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B96" s="14" t="s">
         <v>16</v>
       </c>
@@ -6017,24 +6017,24 @@
       <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="21" width="10.33203125" customWidth="1"/>
-    <col min="22" max="22" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="21" width="10.28515625" customWidth="1"/>
+    <col min="22" max="22" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6045,7 +6045,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -6073,7 +6073,7 @@
       <c r="W3" s="1"/>
       <c r="Y3" s="1"/>
     </row>
-    <row r="4" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -6145,7 +6145,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -6189,7 +6189,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -6227,7 +6227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -6295,7 +6295,7 @@
         <v>6.5454545454545503</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -6333,7 +6333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -6401,7 +6401,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -6439,7 +6439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -6507,7 +6507,7 @@
         <v>0.76</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -6545,7 +6545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -6613,7 +6613,7 @@
         <v>8.61</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -6651,7 +6651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -6689,7 +6689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -6727,7 +6727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -6765,7 +6765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
@@ -6803,7 +6803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>14</v>
       </c>
@@ -6841,7 +6841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>14</v>
       </c>
@@ -6879,7 +6879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>14</v>
       </c>
@@ -6917,7 +6917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>14</v>
       </c>
@@ -6955,7 +6955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>14</v>
       </c>
@@ -6993,7 +6993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>14</v>
       </c>
@@ -7031,7 +7031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>14</v>
       </c>
@@ -7069,7 +7069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="20"/>
       <c r="D26" s="1"/>
@@ -7096,7 +7096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>14</v>
       </c>
@@ -7146,7 +7146,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>14</v>
       </c>
@@ -7190,7 +7190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>14</v>
       </c>
@@ -7264,7 +7264,7 @@
         <v>18.298591494545501</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>14</v>
       </c>
@@ -7308,7 +7308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>14</v>
       </c>
@@ -7333,7 +7333,7 @@
         <v>TCAR*00</v>
       </c>
       <c r="H31" s="22">
-        <v>5.8509000000000002</v>
+        <v>10.5219</v>
       </c>
       <c r="I31" s="22">
         <v>0</v>
@@ -7379,10 +7379,10 @@
       </c>
       <c r="Y31">
         <f t="shared" si="1"/>
-        <v>5.8509000000000002</v>
-      </c>
-    </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.3">
+        <v>10.5219</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>14</v>
       </c>
@@ -7426,7 +7426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>14</v>
       </c>
@@ -7451,7 +7451,7 @@
         <v>TFL*</v>
       </c>
       <c r="H33" s="22">
-        <v>6.7997576454545499</v>
+        <v>13.5995152909091</v>
       </c>
       <c r="I33" s="22">
         <v>0</v>
@@ -7497,10 +7497,10 @@
       </c>
       <c r="Y33">
         <f t="shared" si="1"/>
-        <v>6.7997576454545499</v>
-      </c>
-    </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
+        <v>13.5995152909091</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>14</v>
       </c>
@@ -7544,7 +7544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>14</v>
       </c>
@@ -7618,7 +7618,7 @@
         <v>24.7878803309091</v>
       </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>14</v>
       </c>
@@ -7662,7 +7662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>14</v>
       </c>
@@ -7706,7 +7706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>14</v>
       </c>
@@ -7750,7 +7750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>14</v>
       </c>
@@ -7794,7 +7794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>14</v>
       </c>
@@ -7838,7 +7838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>14</v>
       </c>
@@ -7882,7 +7882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>14</v>
       </c>
@@ -7926,7 +7926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>14</v>
       </c>
@@ -7970,7 +7970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>14</v>
       </c>
@@ -8014,7 +8014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>14</v>
       </c>
@@ -8058,7 +8058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>14</v>
       </c>
@@ -8102,7 +8102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Added missing stock data and Pkm/Tkm data to BY-file
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_B-NewTechs_TRA_Trans.xlsx
+++ b/SubRES_TMPL/SubRes_B-NewTechs_TRA_Trans.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GabGren\Work Folders\Documents\TransportElModellSthlm\SimpleModel\City_TRA_STHLM\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GabGren\Work Folders\Documents\TransportElModellSthlm\SimpleModel\City_TRA_STHLM_ts\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FC893F4-0864-4DD6-A013-5A15D1B5DB21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E75C2FC4-FA66-4FBF-A66C-E93A3678C7C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1425" windowWidth="28800" windowHeight="15375" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="44685" yWindow="3645" windowWidth="28800" windowHeight="15045" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Param_Transformation" sheetId="3" r:id="rId1"/>
@@ -3966,7 +3966,7 @@
       </c>
       <c r="F12" s="12">
         <f>FILL!Y11</f>
-        <v>0.76</v>
+        <v>0.10390000000000001</v>
       </c>
       <c r="G12" s="1" t="str">
         <f>FILL!G11&amp;",-*00"</f>
@@ -4018,7 +4018,7 @@
       </c>
       <c r="F14" s="12">
         <f>FILL!Y13</f>
-        <v>8.61</v>
+        <v>6.7</v>
       </c>
       <c r="G14" s="1" t="str">
         <f>FILL!G13&amp;",-*00"</f>
@@ -4484,7 +4484,7 @@
       </c>
       <c r="F32" s="25">
         <f>FILL!Y31</f>
-        <v>10.5219</v>
+        <v>5.9874210000000003</v>
       </c>
       <c r="G32" s="24" t="s">
         <v>65</v>
@@ -4538,7 +4538,7 @@
       </c>
       <c r="F34" s="25">
         <f>FILL!Y33</f>
-        <v>13.5995152909091</v>
+        <v>9.1937820909090906</v>
       </c>
       <c r="G34" s="1" t="str">
         <f>FILL!G33&amp;",-*00"</f>
@@ -4594,7 +4594,7 @@
       </c>
       <c r="F36" s="17">
         <f>FILL!Y35</f>
-        <v>24.7878803309091</v>
+        <v>7.6864538008824699</v>
       </c>
       <c r="G36" s="1" t="str">
         <f>FILL!G35&amp;",-*00"</f>
@@ -5173,7 +5173,7 @@
       <c r="E60" s="1"/>
       <c r="F60" s="12">
         <f t="shared" ref="F60:G60" si="9">F12</f>
-        <v>0.76</v>
+        <v>0.10390000000000001</v>
       </c>
       <c r="G60" s="1" t="str">
         <f t="shared" si="9"/>
@@ -5219,7 +5219,7 @@
       <c r="E62" s="1"/>
       <c r="F62" s="12">
         <f t="shared" ref="F62:G62" si="11">F14</f>
-        <v>8.61</v>
+        <v>6.7</v>
       </c>
       <c r="G62" s="1" t="str">
         <f t="shared" si="11"/>
@@ -5624,7 +5624,7 @@
       <c r="E80" s="16"/>
       <c r="F80" s="17">
         <f t="shared" ref="F80:G80" si="29">F32</f>
-        <v>10.5219</v>
+        <v>5.9874210000000003</v>
       </c>
       <c r="G80" s="1" t="str">
         <f t="shared" si="29"/>
@@ -5670,7 +5670,7 @@
       <c r="E82" s="16"/>
       <c r="F82" s="17">
         <f t="shared" ref="F82:G82" si="31">F34</f>
-        <v>13.5995152909091</v>
+        <v>9.1937820909090906</v>
       </c>
       <c r="G82" s="1" t="str">
         <f t="shared" si="31"/>
@@ -5716,7 +5716,7 @@
       <c r="E84" s="16"/>
       <c r="F84" s="17">
         <f t="shared" ref="F84:G84" si="33">F36</f>
-        <v>24.7878803309091</v>
+        <v>7.6864538008824699</v>
       </c>
       <c r="G84" s="1" t="str">
         <f t="shared" si="33"/>
@@ -6458,7 +6458,7 @@
         <v>46</v>
       </c>
       <c r="H11" s="22">
-        <v>0.76</v>
+        <v>0.10390000000000001</v>
       </c>
       <c r="I11" s="22">
         <v>0</v>
@@ -6504,7 +6504,7 @@
       </c>
       <c r="Y11">
         <f t="shared" si="1"/>
-        <v>0.76</v>
+        <v>0.10390000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
@@ -6564,7 +6564,7 @@
         <v>48</v>
       </c>
       <c r="H13" s="22">
-        <v>8.61</v>
+        <v>6.7</v>
       </c>
       <c r="I13" s="22">
         <v>0</v>
@@ -6610,7 +6610,7 @@
       </c>
       <c r="Y13">
         <f t="shared" si="1"/>
-        <v>8.61</v>
+        <v>6.7</v>
       </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
@@ -7333,7 +7333,7 @@
         <v>TCAR*00</v>
       </c>
       <c r="H31" s="22">
-        <v>10.5219</v>
+        <v>5.9874210000000003</v>
       </c>
       <c r="I31" s="22">
         <v>0</v>
@@ -7379,7 +7379,7 @@
       </c>
       <c r="Y31">
         <f t="shared" si="1"/>
-        <v>10.5219</v>
+        <v>5.9874210000000003</v>
       </c>
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.25">
@@ -7451,7 +7451,7 @@
         <v>TFL*</v>
       </c>
       <c r="H33" s="22">
-        <v>13.5995152909091</v>
+        <v>9.1937820909090906</v>
       </c>
       <c r="I33" s="22">
         <v>0</v>
@@ -7497,7 +7497,7 @@
       </c>
       <c r="Y33">
         <f t="shared" si="1"/>
-        <v>13.5995152909091</v>
+        <v>9.1937820909090906</v>
       </c>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.25">
@@ -7569,7 +7569,7 @@
         <v>TFR*</v>
       </c>
       <c r="H35" s="22">
-        <v>24.7878803309091</v>
+        <v>7.6864538008824699</v>
       </c>
       <c r="I35" s="22">
         <v>0</v>
@@ -7615,7 +7615,7 @@
       </c>
       <c r="Y35">
         <f t="shared" si="1"/>
-        <v>24.7878803309091</v>
+        <v>7.6864538008824699</v>
       </c>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.25">

</xml_diff>